<commit_message>
reducing space of figures
</commit_message>
<xml_diff>
--- a/eval/resultPietro.xlsx
+++ b/eval/resultPietro.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26221"/>
   <workbookPr filterPrivacy="1" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13040" tabRatio="730" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13940" tabRatio="730" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="case2_varyIter" sheetId="1" r:id="rId1"/>
@@ -794,11 +794,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2133165672"/>
-        <c:axId val="2133162680"/>
+        <c:axId val="2140852744"/>
+        <c:axId val="2139296632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2133165672"/>
+        <c:axId val="2140852744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -807,7 +807,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2133162680"/>
+        <c:crossAx val="2139296632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -815,7 +815,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2133162680"/>
+        <c:axId val="2139296632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -828,7 +828,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2133165672"/>
+        <c:crossAx val="2140852744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1168,11 +1168,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2130730776"/>
-        <c:axId val="2130727784"/>
+        <c:axId val="2142182632"/>
+        <c:axId val="2142185608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2130730776"/>
+        <c:axId val="2142182632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1181,7 +1181,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2130727784"/>
+        <c:crossAx val="2142185608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1189,7 +1189,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2130727784"/>
+        <c:axId val="2142185608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1202,7 +1202,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2130730776"/>
+        <c:crossAx val="2142182632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1457,11 +1457,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2134367560"/>
-        <c:axId val="2134370600"/>
+        <c:axId val="2142217688"/>
+        <c:axId val="2142220776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2134367560"/>
+        <c:axId val="2142217688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1476,12 +1476,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200"/>
+              <a:defRPr sz="1400"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2134370600"/>
+        <c:crossAx val="2142220776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1489,7 +1489,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2134370600"/>
+        <c:axId val="2142220776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.4"/>
@@ -1507,12 +1507,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200"/>
+              <a:defRPr sz="1400"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2134367560"/>
+        <c:crossAx val="2142217688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -1979,11 +1979,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2134411256"/>
-        <c:axId val="2134414232"/>
+        <c:axId val="2140984840"/>
+        <c:axId val="2140978648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2134411256"/>
+        <c:axId val="2140984840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1992,7 +1992,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2134414232"/>
+        <c:crossAx val="2140978648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2000,7 +2000,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2134414232"/>
+        <c:axId val="2140978648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.8"/>
@@ -2012,13 +2012,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2134411256"/>
+        <c:crossAx val="2140984840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2338,11 +2339,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2134446600"/>
-        <c:axId val="2134449688"/>
+        <c:axId val="2141030328"/>
+        <c:axId val="2141033416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2134446600"/>
+        <c:axId val="2141030328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2357,12 +2358,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200"/>
+              <a:defRPr sz="1400"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2134449688"/>
+        <c:crossAx val="2141033416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2370,7 +2371,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2134449688"/>
+        <c:axId val="2141033416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.4"/>
@@ -2388,12 +2389,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200"/>
+              <a:defRPr sz="1400"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2134446600"/>
+        <c:crossAx val="2141030328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -2734,11 +2735,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2134491352"/>
-        <c:axId val="2134494440"/>
+        <c:axId val="2141081544"/>
+        <c:axId val="2141084632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2134491352"/>
+        <c:axId val="2141081544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2748,7 +2749,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2134494440"/>
+        <c:crossAx val="2141084632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2756,7 +2757,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2134494440"/>
+        <c:axId val="2141084632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2769,13 +2770,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2134491352"/>
+        <c:crossAx val="2141081544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3023,11 +3025,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2134526344"/>
-        <c:axId val="2134529432"/>
+        <c:axId val="2141116568"/>
+        <c:axId val="2141119656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2134526344"/>
+        <c:axId val="2141116568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3042,12 +3044,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200"/>
+              <a:defRPr sz="1400"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2134529432"/>
+        <c:crossAx val="2141119656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3055,7 +3057,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2134529432"/>
+        <c:axId val="2141119656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.4"/>
@@ -3073,12 +3075,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200"/>
+              <a:defRPr sz="1400"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2134526344"/>
+        <c:crossAx val="2141116568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -3545,11 +3547,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2134570504"/>
-        <c:axId val="2134573480"/>
+        <c:axId val="2139233992"/>
+        <c:axId val="2139231000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2134570504"/>
+        <c:axId val="2139233992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3558,7 +3560,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2134573480"/>
+        <c:crossAx val="2139231000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3566,7 +3568,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2134573480"/>
+        <c:axId val="2139231000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.8"/>
@@ -3578,13 +3580,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2134570504"/>
+        <c:crossAx val="2139233992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3907,11 +3910,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2134606200"/>
-        <c:axId val="2134609288"/>
+        <c:axId val="2141672472"/>
+        <c:axId val="2141669368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2134606200"/>
+        <c:axId val="2141672472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3926,12 +3929,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200"/>
+              <a:defRPr sz="1400"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2134609288"/>
+        <c:crossAx val="2141669368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3939,7 +3942,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2134609288"/>
+        <c:axId val="2141669368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.4"/>
@@ -3957,12 +3960,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200"/>
+              <a:defRPr sz="1400"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2134606200"/>
+        <c:crossAx val="2141672472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -4218,11 +4221,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2133096632"/>
-        <c:axId val="2133093528"/>
+        <c:axId val="2139290744"/>
+        <c:axId val="2139287688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2133096632"/>
+        <c:axId val="2139290744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4237,12 +4240,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200"/>
+              <a:defRPr sz="1400"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2133093528"/>
+        <c:crossAx val="2139287688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4250,7 +4253,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2133093528"/>
+        <c:axId val="2139287688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.4"/>
@@ -4268,12 +4271,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200"/>
+              <a:defRPr sz="1400"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2133096632"/>
+        <c:crossAx val="2139290744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -4700,11 +4703,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2133044264"/>
-        <c:axId val="2133041128"/>
+        <c:axId val="2140951784"/>
+        <c:axId val="2140954920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2133044264"/>
+        <c:axId val="2140951784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4714,12 +4717,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2133041128"/>
+        <c:crossAx val="2140954920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2133041128"/>
+        <c:axId val="2140954920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4730,7 +4733,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2133044264"/>
+        <c:crossAx val="2140951784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5215,11 +5218,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2133000472"/>
-        <c:axId val="2132997480"/>
+        <c:axId val="2142763368"/>
+        <c:axId val="2142758904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2133000472"/>
+        <c:axId val="2142763368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5228,7 +5231,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132997480"/>
+        <c:crossAx val="2142758904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5236,7 +5239,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2132997480"/>
+        <c:axId val="2142758904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.8"/>
@@ -5248,7 +5251,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2133000472"/>
+        <c:crossAx val="2142763368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5575,11 +5578,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2132965400"/>
-        <c:axId val="2132962296"/>
+        <c:axId val="2142811480"/>
+        <c:axId val="2142814568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2132965400"/>
+        <c:axId val="2142811480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5594,12 +5597,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200"/>
+              <a:defRPr sz="1400"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132962296"/>
+        <c:crossAx val="2142814568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5607,7 +5610,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2132962296"/>
+        <c:axId val="2142814568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.4"/>
@@ -5625,12 +5628,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200"/>
+              <a:defRPr sz="1400"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132965400"/>
+        <c:crossAx val="2142811480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -5971,11 +5974,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2132923224"/>
-        <c:axId val="2132920232"/>
+        <c:axId val="2142860248"/>
+        <c:axId val="2142863224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2132923224"/>
+        <c:axId val="2142860248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5984,7 +5987,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132920232"/>
+        <c:crossAx val="2142863224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5992,7 +5995,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2132920232"/>
+        <c:axId val="2142863224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -6005,7 +6008,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132923224"/>
+        <c:crossAx val="2142860248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6260,11 +6263,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2132887896"/>
-        <c:axId val="2132884808"/>
+        <c:axId val="2139371864"/>
+        <c:axId val="2139280968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2132887896"/>
+        <c:axId val="2139371864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6279,12 +6282,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200"/>
+              <a:defRPr sz="1400"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132884808"/>
+        <c:crossAx val="2139280968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6292,7 +6295,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2132884808"/>
+        <c:axId val="2139280968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.4"/>
@@ -6310,12 +6313,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" baseline="0"/>
+              <a:defRPr sz="1400" baseline="0"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2132887896"/>
+        <c:crossAx val="2139371864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -6782,11 +6785,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2132843432"/>
-        <c:axId val="2132840440"/>
+        <c:axId val="2142094504"/>
+        <c:axId val="2142097480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2132843432"/>
+        <c:axId val="2142094504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6795,7 +6798,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132840440"/>
+        <c:crossAx val="2142097480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6803,7 +6806,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2132840440"/>
+        <c:axId val="2142097480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.8"/>
@@ -6815,7 +6818,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132843432"/>
+        <c:crossAx val="2142094504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7142,11 +7145,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2130783432"/>
-        <c:axId val="2130780376"/>
+        <c:axId val="2142133432"/>
+        <c:axId val="2142136520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2130783432"/>
+        <c:axId val="2142133432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7161,12 +7164,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200"/>
+              <a:defRPr sz="1400"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2130780376"/>
+        <c:crossAx val="2142136520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7174,7 +7177,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2130780376"/>
+        <c:axId val="2142136520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.4"/>
@@ -7192,12 +7195,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200"/>
+              <a:defRPr sz="1400"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2130783432"/>
+        <c:crossAx val="2142133432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -8064,7 +8067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -8811,7 +8814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
@@ -10772,7 +10775,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
@@ -12426,8 +12429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>